<commit_message>
update other xls just in case
</commit_message>
<xml_diff>
--- a/data/xlsx/QUEST-Rad.xlsx
+++ b/data/xlsx/QUEST-Rad.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Denis/Documents/Publis/Benchmarks-2025/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Denis/Documents/Publis/Benchmarks-2025/SI-Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F933BD-9C4E-9643-8EBE-FA2DB660F626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D67FAA95-EDF8-C841-9F86-D87C1CEF64D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-220" yWindow="6420" windowWidth="30240" windowHeight="14360" firstSheet="16" activeTab="32" xr2:uid="{243CE0D0-E45B-AE42-9190-660A76D79A56}"/>
+    <workbookView xWindow="0" yWindow="4320" windowWidth="30240" windowHeight="14360" firstSheet="16" activeTab="20" xr2:uid="{243CE0D0-E45B-AE42-9190-660A76D79A56}"/>
   </bookViews>
   <sheets>
     <sheet name="AlCH2" sheetId="34" r:id="rId1"/>
@@ -4455,7 +4455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -4564,7 +4564,6 @@
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -22868,8 +22867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72BAE612-1789-1044-B79C-5BCE2D87687B}">
   <dimension ref="A1:Z32"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23168,11 +23167,11 @@
         <v>1204</v>
       </c>
       <c r="Q5" s="14">
-        <f>L5+M5-J5</f>
+        <f t="shared" ref="Q5:Q8" si="0">L5+M5-J5</f>
         <v>2.093</v>
       </c>
       <c r="R5" s="14">
-        <f>Q5+F5-E5</f>
+        <f t="shared" ref="R5:R8" si="1">Q5+F5-E5</f>
         <v>2.0879999999999996</v>
       </c>
       <c r="S5" s="45" t="s">
@@ -23245,11 +23244,11 @@
         <v>1205</v>
       </c>
       <c r="Q6" s="14">
-        <f>L6+M6-J6</f>
+        <f t="shared" si="0"/>
         <v>5.4549999999999992</v>
       </c>
       <c r="R6" s="14">
-        <f t="shared" ref="R6:R14" si="0">Q6+F6-E6</f>
+        <f t="shared" si="1"/>
         <v>5.4899999999999984</v>
       </c>
       <c r="S6" s="45" t="s">
@@ -23306,7 +23305,9 @@
       <c r="K7" s="14">
         <v>6.1639999999999997</v>
       </c>
-      <c r="L7" s="14"/>
+      <c r="L7" s="14">
+        <v>6.15</v>
+      </c>
       <c r="M7" s="14">
         <v>6.1970000000000001</v>
       </c>
@@ -23320,12 +23321,12 @@
         <v>1219</v>
       </c>
       <c r="Q7" s="14">
-        <f t="shared" ref="Q7:Q14" si="1">I7+K7-H7+M7-J7</f>
-        <v>6.1529999999999987</v>
+        <f t="shared" si="0"/>
+        <v>6.1490000000000009</v>
       </c>
       <c r="R7" s="14">
-        <f t="shared" si="0"/>
-        <v>6.1639999999999988</v>
+        <f t="shared" si="1"/>
+        <v>6.160000000000001</v>
       </c>
       <c r="S7" s="45" t="s">
         <v>986</v>
@@ -23381,7 +23382,9 @@
       <c r="K8" s="14">
         <v>6.2889999999999997</v>
       </c>
-      <c r="L8" s="14"/>
+      <c r="L8" s="14">
+        <v>6.3620000000000001</v>
+      </c>
       <c r="M8" s="14">
         <v>6.3140000000000001</v>
       </c>
@@ -23395,12 +23398,12 @@
         <v>1218</v>
       </c>
       <c r="Q8" s="14">
+        <f t="shared" si="0"/>
+        <v>6.3609999999999998</v>
+      </c>
+      <c r="R8" s="14">
         <f t="shared" si="1"/>
-        <v>6.3649999999999993</v>
-      </c>
-      <c r="R8" s="14">
-        <f t="shared" si="0"/>
-        <v>6.3719999999999999</v>
+        <v>6.3679999999999986</v>
       </c>
       <c r="S8" s="5"/>
       <c r="T8" s="5" t="s">
@@ -23540,7 +23543,7 @@
         <v>6.9300000000000006</v>
       </c>
       <c r="R10" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="R10:R14" si="2">Q10+F10-E10</f>
         <v>6.883</v>
       </c>
       <c r="S10" s="5"/>
@@ -23595,7 +23598,7 @@
       <c r="K11" s="14">
         <v>7.17</v>
       </c>
-      <c r="L11" s="66">
+      <c r="L11" s="14">
         <v>7.077</v>
       </c>
       <c r="M11" s="14">
@@ -23615,7 +23618,7 @@
         <v>7.0769999999999991</v>
       </c>
       <c r="R11" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.0779999999999994</v>
       </c>
       <c r="S11" s="45" t="s">
@@ -23690,7 +23693,7 @@
         <v>7.7370000000000001</v>
       </c>
       <c r="R12" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.7289999999999992</v>
       </c>
       <c r="S12" s="45" t="s">
@@ -23749,7 +23752,9 @@
       <c r="K13" s="14">
         <v>6.3879999999999999</v>
       </c>
-      <c r="L13" s="21"/>
+      <c r="L13" s="38">
+        <v>6.3789999999999996</v>
+      </c>
       <c r="M13" s="14">
         <v>6.3890000000000002</v>
       </c>
@@ -23763,12 +23768,12 @@
         <v>1206</v>
       </c>
       <c r="Q13" s="14">
-        <f t="shared" si="1"/>
-        <v>6.3919999999999995</v>
+        <f>L13+M13-J13</f>
+        <v>6.3740000000000006</v>
       </c>
       <c r="R13" s="14">
-        <f t="shared" si="0"/>
-        <v>6.4069999999999991</v>
+        <f t="shared" si="2"/>
+        <v>6.3890000000000002</v>
       </c>
       <c r="S13" s="45" t="s">
         <v>990</v>
@@ -23822,7 +23827,7 @@
       <c r="K14" s="14">
         <v>6.758</v>
       </c>
-      <c r="L14" s="14"/>
+      <c r="L14" s="22"/>
       <c r="M14" s="14">
         <v>6.7569999999999997</v>
       </c>
@@ -23836,11 +23841,11 @@
         <v>1207</v>
       </c>
       <c r="Q14" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="Q13:Q14" si="3">I14+K14-H14+M14-J14</f>
         <v>6.7629999999999999</v>
       </c>
       <c r="R14" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.778999999999999</v>
       </c>
       <c r="S14" s="45" t="s">
@@ -23991,7 +23996,7 @@
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
       <c r="B20" s="12" t="str">
-        <f t="shared" ref="B20:B26" si="2">B6</f>
+        <f t="shared" ref="B20:B26" si="4">B6</f>
         <v>A' (Ryd, n-R)</v>
       </c>
       <c r="C20" s="14">
@@ -24022,7 +24027,7 @@
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
       <c r="B21" s="12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>A' (Mix)</v>
       </c>
       <c r="C21" s="14">
@@ -24053,7 +24058,7 @@
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
       <c r="B22" s="12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>A' (Ryd, n-R)</v>
       </c>
       <c r="C22" s="14">
@@ -24084,7 +24089,7 @@
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>A' (Ryd, n-R)</v>
       </c>
       <c r="C23" s="14">
@@ -24115,7 +24120,7 @@
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
       <c r="B24" s="12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>A" (Mix)</v>
       </c>
       <c r="C24" s="14">
@@ -24146,7 +24151,7 @@
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
       <c r="B25" s="12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>A" (Mix)</v>
       </c>
       <c r="C25" s="14">
@@ -24177,7 +24182,7 @@
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="6"/>
       <c r="B26" s="12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>A" (Val, n-pi*)</v>
       </c>
       <c r="C26" s="14">
@@ -24211,7 +24216,7 @@
         <v>Quartet</v>
       </c>
       <c r="B27" s="12" t="str">
-        <f t="shared" ref="B27:B28" si="3">B13</f>
+        <f t="shared" ref="B27:B28" si="5">B13</f>
         <v>A" (Val, n-pi*)</v>
       </c>
       <c r="C27" s="14">
@@ -24242,7 +24247,7 @@
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
       <c r="B28" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>A' (Val, pi-pi*)</v>
       </c>
       <c r="C28" s="14">
@@ -33957,7 +33962,7 @@
   <dimension ref="A1:T32"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R43" sqref="R43"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -34533,9 +34538,12 @@
       <c r="H12" s="14">
         <v>6.6319999999999997</v>
       </c>
+      <c r="I12" s="14">
+        <v>6.6459999999999999</v>
+      </c>
       <c r="K12" s="14">
-        <f>H12</f>
-        <v>6.6319999999999997</v>
+        <f t="shared" si="0"/>
+        <v>6.5089999999999986</v>
       </c>
       <c r="M12" s="5"/>
       <c r="N12" s="17" t="s">
@@ -42810,7 +42818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F82C8F-7CA1-3448-936B-25FA27123626}">
   <dimension ref="A1:X33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="K18" sqref="K18:S19"/>
     </sheetView>
   </sheetViews>

</xml_diff>